<commit_message>
BUGFIX: Dropbox now shares also UIImage, which is properly converted to file
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="44">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>SHKURLContentTypeAudio SHKURLContentTypeVideo SHKURLContentTypeImage SHKURLContentTypeWebpage</t>
-  </si>
-  <si>
-    <t>as description</t>
   </si>
   <si>
     <t>Prefilled means, that values of these properties are prefilled as default text in share edit dialogue, or shared if autoshare is on.</t>
@@ -145,9 +142,6 @@
   </si>
   <si>
     <t>video, audio, image</t>
-  </si>
-  <si>
-    <t>item.data (file type)</t>
   </si>
   <si>
     <t>It is mandatory for each sharer that it can handle these basic share properties. Also it is mandatory for successful share to prefill these.</t>
@@ -188,9 +182,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>as comment</t>
-  </si>
-  <si>
     <t>Twitter</t>
   </si>
   <si>
@@ -207,6 +198,36 @@
   </si>
   <si>
     <t>STILL INCOMPLETE!!!</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>caption</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>item.file (file type)</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>SHKShareTypeUserInfo</t>
+  </si>
+  <si>
+    <t>Dropbox</t>
   </si>
 </sst>
 </file>
@@ -302,7 +323,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -334,8 +355,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -367,8 +392,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -384,6 +410,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -399,6 +427,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,10 +758,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X79"/>
+  <dimension ref="A1:X80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <pane ySplit="1460" topLeftCell="A43" activePane="bottomLeft"/>
+      <selection activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -746,12 +778,12 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -817,22 +849,22 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:24">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:24">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:24" s="5" customFormat="1">
@@ -843,25 +875,31 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>35</v>
+      <c r="K14" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:24" s="9" customFormat="1">
@@ -877,7 +915,9 @@
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="K15" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -919,7 +959,9 @@
       <c r="I16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1023,7 +1065,9 @@
       <c r="I19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1044,10 +1088,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1057,7 +1101,9 @@
         <v>5</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1166,10 +1212,10 @@
     </row>
     <row r="24" spans="1:24">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1196,7 +1242,7 @@
     </row>
     <row r="25" spans="1:24">
       <c r="B25" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1252,7 +1298,7 @@
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -1261,7 +1307,9 @@
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="K27" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
@@ -1423,7 +1471,9 @@
       <c r="I32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -1528,10 +1578,10 @@
     </row>
     <row r="36" spans="1:23">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1557,7 +1607,7 @@
     </row>
     <row r="37" spans="1:23">
       <c r="B37" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1611,18 +1661,18 @@
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
+      <c r="K39" s="11"/>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
@@ -1720,8 +1770,12 @@
       <c r="I42" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
+      <c r="J42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
@@ -1759,7 +1813,9 @@
       <c r="I43" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J43" s="1"/>
+      <c r="J43" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -1786,7 +1842,9 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="J44" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -1891,10 +1949,10 @@
     </row>
     <row r="48" spans="1:23">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1920,7 +1978,7 @@
     </row>
     <row r="49" spans="1:23">
       <c r="B49" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1974,25 +2032,25 @@
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
@@ -2104,7 +2162,9 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
+      <c r="J55" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
@@ -2131,7 +2191,9 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
+      <c r="J56" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -2177,10 +2239,10 @@
     </row>
     <row r="58" spans="1:23">
       <c r="A58" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2189,8 +2251,12 @@
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
+      <c r="J58" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
@@ -2230,10 +2296,10 @@
     </row>
     <row r="60" spans="1:23">
       <c r="A60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -2259,7 +2325,7 @@
     </row>
     <row r="61" spans="1:23">
       <c r="B61" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2307,29 +2373,52 @@
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
     </row>
-    <row r="63" spans="1:23">
-      <c r="B63" s="3"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1"/>
-      <c r="U63" s="1"/>
-      <c r="V63" s="1"/>
-      <c r="W63" s="1"/>
+    <row r="63" spans="1:23" s="9" customFormat="1">
+      <c r="A63" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J63" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K63" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L63" s="8"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="8"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="8"/>
+      <c r="R63" s="8"/>
+      <c r="S63" s="8"/>
+      <c r="T63" s="8"/>
+      <c r="U63" s="8"/>
+      <c r="V63" s="8"/>
+      <c r="W63" s="8"/>
     </row>
     <row r="64" spans="1:23">
       <c r="B64" s="3"/>
@@ -2715,6 +2804,30 @@
       <c r="V79" s="1"/>
       <c r="W79" s="1"/>
     </row>
+    <row r="80" spans="2:23">
+      <c r="B80" s="3"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+      <c r="W80" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
NEW FEATURE: SHKMail made more universal (issue #704) + property support matrix update
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="45">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Dropbox</t>
+  </si>
+  <si>
+    <t>Mail</t>
   </si>
 </sst>
 </file>
@@ -760,10 +763,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <pane ySplit="1460" topLeftCell="A43" activePane="bottomLeft"/>
-      <selection activeCell="K15" sqref="K15"/>
-      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4160" topLeftCell="A14"/>
+      <selection activeCell="L35" sqref="L35"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -901,6 +904,9 @@
       <c r="K14" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="L14" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:24" s="9" customFormat="1">
       <c r="A15" s="6" t="s">
@@ -963,7 +969,9 @@
         <v>5</v>
       </c>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="L16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1027,7 +1035,9 @@
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1069,7 +1079,9 @@
         <v>5</v>
       </c>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1102,10 +1114,12 @@
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1171,7 +1185,9 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -1341,9 +1357,13 @@
       <c r="I28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="L28" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -1403,7 +1423,9 @@
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
+      <c r="L30" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -1432,7 +1454,9 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
+      <c r="L31" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -1475,7 +1499,9 @@
         <v>5</v>
       </c>
       <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
+      <c r="L32" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -1510,7 +1536,9 @@
       <c r="I33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -1539,7 +1567,9 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
+      <c r="L34" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -1706,7 +1736,9 @@
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
+      <c r="L40" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -1776,7 +1808,9 @@
       <c r="K42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L42" s="1"/>
+      <c r="L42" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
@@ -1817,7 +1851,9 @@
         <v>38</v>
       </c>
       <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
+      <c r="L43" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
@@ -1846,7 +1882,9 @@
         <v>35</v>
       </c>
       <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
+      <c r="L44" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
@@ -1910,7 +1948,9 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
+      <c r="L46" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -2081,7 +2121,9 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
+      <c r="L52" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -2135,7 +2177,9 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
+      <c r="L54" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
@@ -2166,7 +2210,9 @@
         <v>39</v>
       </c>
       <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
+      <c r="L55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
@@ -2195,7 +2241,9 @@
         <v>37</v>
       </c>
       <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
+      <c r="L56" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
@@ -2257,7 +2305,9 @@
       <c r="K58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L58" s="1"/>
+      <c r="L58" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
@@ -2407,7 +2457,9 @@
       <c r="K63" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="L63" s="8"/>
+      <c r="L63" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="M63" s="8"/>
       <c r="N63" s="8"/>
       <c r="O63" s="8"/>

</xml_diff>

<commit_message>
REFACTORING: SHKBuffer now uses send method instead of show + SHKSharer cleanup
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -24,6 +24,30 @@
     <author>Vilém Kurz</author>
   </authors>
   <commentList>
+    <comment ref="M19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Vilém Kurz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+either text or title</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B20" authorId="0">
       <text>
         <r>
@@ -48,12 +72,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="M20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Vilém Kurz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+either text or title</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="46">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -231,6 +279,9 @@
   </si>
   <si>
     <t>Mail</t>
+  </si>
+  <si>
+    <t>Buffer</t>
   </si>
 </sst>
 </file>
@@ -326,8 +377,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -397,7 +450,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -415,6 +468,7 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -432,6 +486,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -764,9 +819,9 @@
   <dimension ref="A1:X80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4160" topLeftCell="A14"/>
+      <pane ySplit="4160" topLeftCell="A2" activePane="bottomLeft"/>
       <selection activeCell="L35" sqref="L35"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -907,6 +962,9 @@
       <c r="L14" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="M14" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:24" s="9" customFormat="1">
       <c r="A15" s="6" t="s">
@@ -972,7 +1030,9 @@
       <c r="L16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M16" s="1"/>
+      <c r="M16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1082,7 +1142,9 @@
       <c r="L19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M19" s="1"/>
+      <c r="M19" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1120,7 +1182,9 @@
       <c r="L20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M20" s="1"/>
+      <c r="M20" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1502,7 +1566,9 @@
       <c r="L32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M32" s="1"/>
+      <c r="M32" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -1704,7 +1770,9 @@
       <c r="J39" s="8"/>
       <c r="K39" s="11"/>
       <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
+      <c r="M39" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="N39" s="8"/>
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
@@ -2095,7 +2163,9 @@
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
+      <c r="M51" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="N51" s="8"/>
       <c r="O51" s="8"/>
       <c r="P51" s="8"/>
@@ -2460,7 +2530,9 @@
       <c r="L63" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M63" s="8"/>
+      <c r="M63" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="N63" s="8"/>
       <c r="O63" s="8"/>
       <c r="P63" s="8"/>

</xml_diff>

<commit_message>
NEW FEATURE: file share now has its own icon with file extension in SHKFormFieldCellLargeText
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="50">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -282,6 +282,18 @@
   </si>
   <si>
     <t>Buffer</t>
+  </si>
+  <si>
+    <t>qualifier</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>public</t>
   </si>
 </sst>
 </file>
@@ -377,8 +389,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -450,7 +464,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -469,6 +483,7 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -487,6 +502,7 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -819,9 +835,9 @@
   <dimension ref="A1:X80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4160" topLeftCell="A2" activePane="bottomLeft"/>
+      <pane ySplit="4160" topLeftCell="A24" activePane="bottomLeft"/>
       <selection activeCell="L35" sqref="L35"/>
-      <selection pane="bottomLeft" activeCell="M64" sqref="M64"/>
+      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -965,6 +981,9 @@
       <c r="M14" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="N14" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" spans="1:24" s="9" customFormat="1">
       <c r="A15" s="6" t="s">
@@ -1033,7 +1052,9 @@
       <c r="M16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N16" s="1"/>
+      <c r="N16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -1145,7 +1166,9 @@
       <c r="M19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N19" s="1"/>
+      <c r="N19" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -1185,7 +1208,9 @@
       <c r="M20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -1298,7 +1323,9 @@
         <v>19</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1308,7 +1335,9 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
+      <c r="N24" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -1325,7 +1354,9 @@
         <v>21</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1569,7 +1600,9 @@
       <c r="M32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N32" s="1"/>
+      <c r="N32" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -1680,7 +1713,9 @@
         <v>19</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -1690,7 +1725,9 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
+      <c r="N36" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -1706,7 +1743,9 @@
         <v>21</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1773,7 +1812,9 @@
       <c r="M39" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N39" s="8"/>
+      <c r="N39" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
       <c r="Q39" s="8"/>
@@ -2063,7 +2104,9 @@
         <v>19</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -2089,7 +2132,9 @@
         <v>21</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2166,7 +2211,9 @@
       <c r="M51" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N51" s="8"/>
+      <c r="N51" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="O51" s="8"/>
       <c r="P51" s="8"/>
       <c r="Q51" s="8"/>
@@ -2504,7 +2551,7 @@
         <v>27</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>5</v>
@@ -2533,7 +2580,9 @@
       <c r="M63" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N63" s="8"/>
+      <c r="N63" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="O63" s="8"/>
       <c r="P63" s="8"/>
       <c r="Q63" s="8"/>

</xml_diff>

<commit_message>
NEW FEATURE: SHKTwitter can share media files automatically shared via frog. This means you can share videos and photos larger than 3mb too. Files accepted by Twitter are still uploaded directly to Twitter (photos smaller than 3mb)
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="51">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>public</t>
+  </si>
+  <si>
+    <t>video, image</t>
   </si>
 </sst>
 </file>
@@ -835,9 +838,9 @@
   <dimension ref="A1:X80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4160" topLeftCell="A24" activePane="bottomLeft"/>
+      <pane ySplit="4160" topLeftCell="A13" activePane="bottomLeft"/>
       <selection activeCell="L35" sqref="L35"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1103,7 +1106,9 @@
       <c r="B18" s="3"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1267,7 +1272,9 @@
       <c r="B22" s="3"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1441,7 +1448,9 @@
       <c r="B28" s="3"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1505,7 +1514,9 @@
       <c r="B30" s="3"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1659,7 +1670,9 @@
       <c r="B34" s="3"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1832,7 +1845,9 @@
       <c r="B40" s="3"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F40" s="10" t="s">
         <v>5</v>
       </c>
@@ -2231,7 +2246,9 @@
       <c r="B52" s="3"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="E52" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -2318,7 +2335,9 @@
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -2382,7 +2401,9 @@
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="E57" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -2411,7 +2432,9 @@
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>

</xml_diff>

<commit_message>
NEW FEATURE: Twitter iOS sharer can send large images and videos via yfrog. BUGFIX: “no account” alert is called after authorisation attempt, to allow for initial authorisation.
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="53">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -297,6 +297,12 @@
   </si>
   <si>
     <t>video, image</t>
+  </si>
+  <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>privacy</t>
   </si>
 </sst>
 </file>
@@ -838,9 +844,9 @@
   <dimension ref="A1:X80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4160" topLeftCell="A13" activePane="bottomLeft"/>
+      <pane ySplit="4160" topLeftCell="A41" activePane="bottomLeft"/>
       <selection activeCell="L35" sqref="L35"/>
-      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
+      <selection pane="bottomLeft" activeCell="O64" sqref="O64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -987,6 +993,9 @@
       <c r="N14" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="O14" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:24" s="9" customFormat="1">
       <c r="A15" s="6" t="s">
@@ -1007,7 +1016,9 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+      <c r="O15" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
@@ -1431,7 +1442,9 @@
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
+      <c r="O27" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
@@ -1828,7 +1841,9 @@
       <c r="N39" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O39" s="8"/>
+      <c r="O39" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="P39" s="8"/>
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
@@ -2351,7 +2366,9 @@
       </c>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
+      <c r="O55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
@@ -2382,7 +2399,9 @@
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
+      <c r="O56" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
@@ -2413,7 +2432,9 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
+      <c r="O57" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
@@ -2450,7 +2471,9 @@
       </c>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
+      <c r="O58" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
@@ -2503,7 +2526,9 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
+      <c r="O60" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -2606,7 +2631,9 @@
       <c r="N63" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O63" s="8"/>
+      <c r="O63" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="P63" s="8"/>
       <c r="Q63" s="8"/>
       <c r="R63" s="8"/>

</xml_diff>

<commit_message>
BUGFIX: Facebook iOS sharer presents alert, when there are not accounts in settings.app DOCUMENTATION: sharer matrix updated
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19460" tabRatio="500"/>
+    <workbookView xWindow="-25600" yWindow="-440" windowWidth="25600" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <author>Vilém Kurz</author>
   </authors>
   <commentList>
-    <comment ref="M19" authorId="0">
+    <comment ref="N19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M20" authorId="0">
+    <comment ref="N20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="55">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -260,9 +260,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>caption</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -303,6 +300,15 @@
   </si>
   <si>
     <t>privacy</t>
+  </si>
+  <si>
+    <t>iOS Facebook</t>
+  </si>
+  <si>
+    <t>pictureURI</t>
+  </si>
+  <si>
+    <t>title</t>
   </si>
 </sst>
 </file>
@@ -398,8 +404,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -473,7 +483,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -493,6 +503,8 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -512,6 +524,8 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -841,12 +855,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X80"/>
+  <dimension ref="A1:Y80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4160" topLeftCell="A41" activePane="bottomLeft"/>
-      <selection activeCell="L35" sqref="L35"/>
-      <selection pane="bottomLeft" activeCell="O64" sqref="O64"/>
+      <pane ySplit="4160" topLeftCell="A26"/>
+      <selection activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -857,19 +871,20 @@
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -886,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -897,7 +912,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -908,7 +923,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -919,7 +934,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -930,27 +945,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="5" customFormat="1">
+    <row r="14" spans="1:25" s="5" customFormat="1">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
@@ -979,25 +994,28 @@
         <v>32</v>
       </c>
       <c r="J14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="N14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="M14" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="O14" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" s="9" customFormat="1">
+        <v>47</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" s="9" customFormat="1">
       <c r="A15" s="6" t="s">
         <v>0</v>
       </c>
@@ -1010,16 +1028,16 @@
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="8"/>
+      <c r="L15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
-      <c r="O15" s="8" t="s">
+      <c r="O15" s="8"/>
+      <c r="P15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
@@ -1027,8 +1045,9 @@
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
       <c r="W15" s="8"/>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="X15" s="8"/>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1059,17 +1078,19 @@
       <c r="J16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="K16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O16" s="1"/>
+      <c r="O16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -1079,8 +1100,9 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
-    </row>
-    <row r="17" spans="1:24" ht="59" customHeight="1">
+      <c r="Y16" s="1"/>
+    </row>
+    <row r="17" spans="1:25" ht="59" customHeight="1">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1109,8 +1131,9 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
-    </row>
-    <row r="18" spans="1:24">
+      <c r="Y17" s="1"/>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1132,10 +1155,10 @@
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1147,8 +1170,9 @@
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
-    </row>
-    <row r="19" spans="1:24">
+      <c r="Y18" s="1"/>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1173,19 +1197,21 @@
         <v>5</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="1"/>
       <c r="M19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O19" s="1"/>
+      <c r="O19" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -1195,8 +1221,9 @@
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
-    </row>
-    <row r="20" spans="1:24">
+      <c r="Y19" s="1"/>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1217,17 +1244,19 @@
       <c r="J20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="K20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="1"/>
       <c r="M20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O20" s="1"/>
+      <c r="O20" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
@@ -1237,8 +1266,9 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
-    </row>
-    <row r="21" spans="1:24">
+      <c r="Y20" s="1"/>
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1275,8 +1305,9 @@
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
-    </row>
-    <row r="22" spans="1:24">
+      <c r="Y21" s="1"/>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1287,15 +1318,17 @@
         <v>5</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1307,8 +1340,9 @@
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
-    </row>
-    <row r="23" spans="1:24">
+      <c r="Y22" s="1"/>
+    </row>
+    <row r="23" spans="1:25">
       <c r="B23" s="3"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1332,8 +1366,9 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-    </row>
-    <row r="24" spans="1:24">
+      <c r="Y23" s="1"/>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1342,21 +1377,25 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-      <c r="N24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -1366,22 +1405,27 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
-    </row>
-    <row r="25" spans="1:24">
+      <c r="Y24" s="1"/>
+    </row>
+    <row r="25" spans="1:25">
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
+      <c r="J25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1395,8 +1439,9 @@
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
-    </row>
-    <row r="26" spans="1:24">
+      <c r="Y25" s="1"/>
+    </row>
+    <row r="26" spans="1:25">
       <c r="B26" s="3"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1420,8 +1465,9 @@
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
-    </row>
-    <row r="27" spans="1:24" s="9" customFormat="1">
+      <c r="Y26" s="1"/>
+    </row>
+    <row r="27" spans="1:25" s="9" customFormat="1">
       <c r="A27" s="6" t="s">
         <v>1</v>
       </c>
@@ -1436,16 +1482,16 @@
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="11" t="s">
+      <c r="K27" s="8"/>
+      <c r="L27" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
-      <c r="O27" s="8" t="s">
+      <c r="O27" s="8"/>
+      <c r="P27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
@@ -1453,8 +1499,9 @@
       <c r="U27" s="8"/>
       <c r="V27" s="8"/>
       <c r="W27" s="8"/>
-    </row>
-    <row r="28" spans="1:24">
+      <c r="X27" s="8"/>
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1477,11 +1524,13 @@
       <c r="J28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M28" s="1"/>
+      <c r="K28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1492,8 +1541,9 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
-    </row>
-    <row r="29" spans="1:24">
+      <c r="X28" s="1"/>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1519,8 +1569,9 @@
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
-    </row>
-    <row r="30" spans="1:24">
+      <c r="X29" s="1"/>
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -1542,10 +1593,10 @@
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -1556,8 +1607,9 @@
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
-    </row>
-    <row r="31" spans="1:24">
+      <c r="X30" s="1"/>
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1571,12 +1623,16 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M31" s="1"/>
+      <c r="J31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1587,8 +1643,9 @@
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
-    </row>
-    <row r="32" spans="1:24">
+      <c r="X31" s="1"/>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1617,17 +1674,19 @@
       <c r="J32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="K32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L32" s="1"/>
       <c r="M32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O32" s="1"/>
+      <c r="O32" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -1636,8 +1695,9 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
-    </row>
-    <row r="33" spans="1:23">
+      <c r="X32" s="1"/>
+    </row>
+    <row r="33" spans="1:24">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1659,9 +1719,7 @@
       <c r="I33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -1675,8 +1733,9 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
-    </row>
-    <row r="34" spans="1:23">
+      <c r="X33" s="1"/>
+    </row>
+    <row r="34" spans="1:24">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1687,15 +1746,17 @@
         <v>5</v>
       </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -1706,8 +1767,9 @@
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
-    </row>
-    <row r="35" spans="1:23">
+      <c r="X34" s="1"/>
+    </row>
+    <row r="35" spans="1:24">
       <c r="B35" s="3"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1730,8 +1792,9 @@
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-    </row>
-    <row r="36" spans="1:23">
+      <c r="X35" s="1"/>
+    </row>
+    <row r="36" spans="1:24">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1740,21 +1803,25 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
+      <c r="J36" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-      <c r="N36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
@@ -1763,22 +1830,27 @@
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-    </row>
-    <row r="37" spans="1:23">
+      <c r="X36" s="1"/>
+    </row>
+    <row r="37" spans="1:24">
       <c r="B37" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
+      <c r="J37" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -1791,8 +1863,9 @@
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
-    </row>
-    <row r="38" spans="1:23">
+      <c r="X37" s="1"/>
+    </row>
+    <row r="38" spans="1:24">
       <c r="B38" s="3"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1815,8 +1888,9 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
-    </row>
-    <row r="39" spans="1:23" s="9" customFormat="1">
+      <c r="X38" s="1"/>
+    </row>
+    <row r="39" spans="1:24" s="9" customFormat="1">
       <c r="A39" s="6" t="s">
         <v>3</v>
       </c>
@@ -1833,18 +1907,18 @@
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="K39" s="8"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="8"/>
       <c r="N39" s="8" t="s">
         <v>27</v>
       </c>
       <c r="O39" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P39" s="8"/>
+      <c r="P39" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
@@ -1852,8 +1926,9 @@
       <c r="U39" s="8"/>
       <c r="V39" s="8"/>
       <c r="W39" s="8"/>
-    </row>
-    <row r="40" spans="1:23">
+      <c r="X39" s="8"/>
+    </row>
+    <row r="40" spans="1:24">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1873,12 +1948,12 @@
       <c r="I40" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="1"/>
+      <c r="J40" s="10"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -1889,8 +1964,9 @@
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
-    </row>
-    <row r="41" spans="1:23">
+      <c r="X40" s="1"/>
+    </row>
+    <row r="41" spans="1:24">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1902,7 +1978,7 @@
       <c r="G41" s="10"/>
       <c r="H41" s="1"/>
       <c r="I41" s="10"/>
-      <c r="J41" s="1"/>
+      <c r="J41" s="10"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -1916,8 +1992,9 @@
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
-    </row>
-    <row r="42" spans="1:23">
+      <c r="X41" s="1"/>
+    </row>
+    <row r="42" spans="1:24">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -1941,7 +2018,7 @@
       <c r="I42" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J42" s="10" t="s">
         <v>5</v>
       </c>
       <c r="K42" s="1" t="s">
@@ -1950,7 +2027,9 @@
       <c r="L42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M42" s="1"/>
+      <c r="M42" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -1961,8 +2040,9 @@
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
-    </row>
-    <row r="43" spans="1:23">
+      <c r="X42" s="1"/>
+    </row>
+    <row r="43" spans="1:24">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1986,14 +2066,16 @@
       <c r="I43" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M43" s="1"/>
+      <c r="J43" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -2004,8 +2086,9 @@
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
-    </row>
-    <row r="44" spans="1:23">
+      <c r="X43" s="1"/>
+    </row>
+    <row r="44" spans="1:24">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2017,14 +2100,12 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="L44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -2035,8 +2116,9 @@
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
-    </row>
-    <row r="45" spans="1:23">
+      <c r="X44" s="1"/>
+    </row>
+    <row r="45" spans="1:24">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -2072,8 +2154,9 @@
       <c r="U45" s="1"/>
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
-    </row>
-    <row r="46" spans="1:23">
+      <c r="X45" s="1"/>
+    </row>
+    <row r="46" spans="1:24">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2087,10 +2170,10 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
@@ -2101,8 +2184,9 @@
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
-    </row>
-    <row r="47" spans="1:23">
+      <c r="X46" s="1"/>
+    </row>
+    <row r="47" spans="1:24">
       <c r="B47" s="3"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2125,8 +2209,9 @@
       <c r="U47" s="1"/>
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
-    </row>
-    <row r="48" spans="1:23">
+      <c r="X47" s="1"/>
+    </row>
+    <row r="48" spans="1:24">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -2135,7 +2220,7 @@
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2156,14 +2241,15 @@
       <c r="U48" s="1"/>
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
-    </row>
-    <row r="49" spans="1:23">
+      <c r="X48" s="1"/>
+    </row>
+    <row r="49" spans="1:24">
       <c r="B49" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2184,8 +2270,9 @@
       <c r="U49" s="1"/>
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
-    </row>
-    <row r="50" spans="1:23">
+      <c r="X49" s="1"/>
+    </row>
+    <row r="50" spans="1:24">
       <c r="B50" s="3"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2208,8 +2295,9 @@
       <c r="U50" s="1"/>
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
-    </row>
-    <row r="51" spans="1:23" s="9" customFormat="1">
+      <c r="X50" s="1"/>
+    </row>
+    <row r="51" spans="1:24" s="9" customFormat="1">
       <c r="A51" s="6" t="s">
         <v>4</v>
       </c>
@@ -2238,13 +2326,13 @@
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
-      <c r="M51" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="M51" s="8"/>
       <c r="N51" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O51" s="8"/>
+      <c r="O51" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="P51" s="8"/>
       <c r="Q51" s="8"/>
       <c r="R51" s="8"/>
@@ -2253,8 +2341,9 @@
       <c r="U51" s="8"/>
       <c r="V51" s="8"/>
       <c r="W51" s="8"/>
-    </row>
-    <row r="52" spans="1:23">
+      <c r="X51" s="8"/>
+    </row>
+    <row r="52" spans="1:24">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -2265,15 +2354,17 @@
         <v>5</v>
       </c>
       <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="G52" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="L52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
@@ -2284,8 +2375,9 @@
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
-    </row>
-    <row r="53" spans="1:23">
+      <c r="X52" s="1"/>
+    </row>
+    <row r="53" spans="1:24">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2311,8 +2403,9 @@
       <c r="U53" s="1"/>
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
-    </row>
-    <row r="54" spans="1:23">
+      <c r="X53" s="1"/>
+    </row>
+    <row r="54" spans="1:24">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -2326,10 +2419,10 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-      <c r="L54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
@@ -2340,8 +2433,9 @@
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
-    </row>
-    <row r="55" spans="1:23">
+      <c r="X54" s="1"/>
+    </row>
+    <row r="55" spans="1:24">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -2354,22 +2448,26 @@
         <v>5</v>
       </c>
       <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+      <c r="G55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M55" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N55" s="1"/>
-      <c r="O55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
@@ -2377,8 +2475,9 @@
       <c r="U55" s="1"/>
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
-    </row>
-    <row r="56" spans="1:23">
+      <c r="X55" s="1"/>
+    </row>
+    <row r="56" spans="1:24">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -2393,16 +2492,18 @@
       <c r="J56" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M56" s="1"/>
+      <c r="K56" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N56" s="1"/>
-      <c r="O56" s="1" t="s">
+      <c r="O56" s="1"/>
+      <c r="P56" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
@@ -2410,8 +2511,9 @@
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
-    </row>
-    <row r="57" spans="1:23">
+      <c r="X56" s="1"/>
+    </row>
+    <row r="57" spans="1:24">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -2424,7 +2526,9 @@
         <v>5</v>
       </c>
       <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="G57" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
@@ -2432,10 +2536,10 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
-      <c r="O57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
@@ -2443,10 +2547,11 @@
       <c r="U57" s="1"/>
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
-    </row>
-    <row r="58" spans="1:23">
+      <c r="X57" s="1"/>
+    </row>
+    <row r="58" spans="1:24">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>22</v>
@@ -2454,27 +2559,31 @@
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="G58" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M58" s="1"/>
+      <c r="M58" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N58" s="1"/>
-      <c r="O58" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
@@ -2482,8 +2591,9 @@
       <c r="U58" s="1"/>
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
-    </row>
-    <row r="59" spans="1:23">
+      <c r="X58" s="1"/>
+    </row>
+    <row r="59" spans="1:24">
       <c r="B59" s="3"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -2506,8 +2616,9 @@
       <c r="U59" s="1"/>
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
-    </row>
-    <row r="60" spans="1:23">
+      <c r="X59" s="1"/>
+    </row>
+    <row r="60" spans="1:24">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -2526,10 +2637,10 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
-      <c r="O60" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
@@ -2537,8 +2648,9 @@
       <c r="U60" s="1"/>
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
-    </row>
-    <row r="61" spans="1:23">
+      <c r="X60" s="1"/>
+    </row>
+    <row r="61" spans="1:24">
       <c r="B61" s="3" t="s">
         <v>21</v>
       </c>
@@ -2563,8 +2675,9 @@
       <c r="U61" s="1"/>
       <c r="V61" s="1"/>
       <c r="W61" s="1"/>
-    </row>
-    <row r="62" spans="1:23">
+      <c r="X61" s="1"/>
+    </row>
+    <row r="62" spans="1:24">
       <c r="B62" s="3"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2587,10 +2700,11 @@
       <c r="U62" s="1"/>
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
-    </row>
-    <row r="63" spans="1:23" s="9" customFormat="1">
+      <c r="X62" s="1"/>
+    </row>
+    <row r="63" spans="1:24" s="9" customFormat="1">
       <c r="A63" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>5</v>
@@ -2608,7 +2722,7 @@
         <v>27</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="H63" s="11" t="s">
         <v>27</v>
@@ -2616,13 +2730,13 @@
       <c r="I63" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J63" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K63" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L63" s="8" t="s">
+      <c r="J63" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K63" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L63" s="11" t="s">
         <v>27</v>
       </c>
       <c r="M63" s="8" t="s">
@@ -2634,7 +2748,9 @@
       <c r="O63" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P63" s="8"/>
+      <c r="P63" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="Q63" s="8"/>
       <c r="R63" s="8"/>
       <c r="S63" s="8"/>
@@ -2642,8 +2758,9 @@
       <c r="U63" s="8"/>
       <c r="V63" s="8"/>
       <c r="W63" s="8"/>
-    </row>
-    <row r="64" spans="1:23">
+      <c r="X63" s="8"/>
+    </row>
+    <row r="64" spans="1:24">
       <c r="B64" s="3"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2666,8 +2783,9 @@
       <c r="U64" s="1"/>
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
-    </row>
-    <row r="65" spans="2:23">
+      <c r="X64" s="1"/>
+    </row>
+    <row r="65" spans="2:24">
       <c r="B65" s="3"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2690,8 +2808,9 @@
       <c r="U65" s="1"/>
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
-    </row>
-    <row r="66" spans="2:23">
+      <c r="X65" s="1"/>
+    </row>
+    <row r="66" spans="2:24">
       <c r="B66" s="3"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2714,8 +2833,9 @@
       <c r="U66" s="1"/>
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
-    </row>
-    <row r="67" spans="2:23">
+      <c r="X66" s="1"/>
+    </row>
+    <row r="67" spans="2:24">
       <c r="B67" s="3"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2738,8 +2858,9 @@
       <c r="U67" s="1"/>
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
-    </row>
-    <row r="68" spans="2:23">
+      <c r="X67" s="1"/>
+    </row>
+    <row r="68" spans="2:24">
       <c r="B68" s="3"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2762,8 +2883,9 @@
       <c r="U68" s="1"/>
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
-    </row>
-    <row r="69" spans="2:23">
+      <c r="X68" s="1"/>
+    </row>
+    <row r="69" spans="2:24">
       <c r="B69" s="3"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2786,8 +2908,9 @@
       <c r="U69" s="1"/>
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
-    </row>
-    <row r="70" spans="2:23">
+      <c r="X69" s="1"/>
+    </row>
+    <row r="70" spans="2:24">
       <c r="B70" s="3"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2810,8 +2933,9 @@
       <c r="U70" s="1"/>
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
-    </row>
-    <row r="71" spans="2:23">
+      <c r="X70" s="1"/>
+    </row>
+    <row r="71" spans="2:24">
       <c r="B71" s="3"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -2834,8 +2958,9 @@
       <c r="U71" s="1"/>
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
-    </row>
-    <row r="72" spans="2:23">
+      <c r="X71" s="1"/>
+    </row>
+    <row r="72" spans="2:24">
       <c r="B72" s="3"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2858,8 +2983,9 @@
       <c r="U72" s="1"/>
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
-    </row>
-    <row r="73" spans="2:23">
+      <c r="X72" s="1"/>
+    </row>
+    <row r="73" spans="2:24">
       <c r="B73" s="3"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -2882,8 +3008,9 @@
       <c r="U73" s="1"/>
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
-    </row>
-    <row r="74" spans="2:23">
+      <c r="X73" s="1"/>
+    </row>
+    <row r="74" spans="2:24">
       <c r="B74" s="3"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2906,8 +3033,9 @@
       <c r="U74" s="1"/>
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
-    </row>
-    <row r="75" spans="2:23">
+      <c r="X74" s="1"/>
+    </row>
+    <row r="75" spans="2:24">
       <c r="B75" s="3"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2930,8 +3058,9 @@
       <c r="U75" s="1"/>
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
-    </row>
-    <row r="76" spans="2:23">
+      <c r="X75" s="1"/>
+    </row>
+    <row r="76" spans="2:24">
       <c r="B76" s="3"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2954,8 +3083,9 @@
       <c r="U76" s="1"/>
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
-    </row>
-    <row r="77" spans="2:23">
+      <c r="X76" s="1"/>
+    </row>
+    <row r="77" spans="2:24">
       <c r="B77" s="3"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2978,8 +3108,9 @@
       <c r="U77" s="1"/>
       <c r="V77" s="1"/>
       <c r="W77" s="1"/>
-    </row>
-    <row r="78" spans="2:23">
+      <c r="X77" s="1"/>
+    </row>
+    <row r="78" spans="2:24">
       <c r="B78" s="3"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -3002,8 +3133,9 @@
       <c r="U78" s="1"/>
       <c r="V78" s="1"/>
       <c r="W78" s="1"/>
-    </row>
-    <row r="79" spans="2:23">
+      <c r="X78" s="1"/>
+    </row>
+    <row r="79" spans="2:24">
       <c r="B79" s="3"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3026,8 +3158,9 @@
       <c r="U79" s="1"/>
       <c r="V79" s="1"/>
       <c r="W79" s="1"/>
-    </row>
-    <row r="80" spans="2:23">
+      <c r="X79" s="1"/>
+    </row>
+    <row r="80" spans="2:24">
       <c r="B80" s="3"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -3050,6 +3183,7 @@
       <c r="U80" s="1"/>
       <c r="V80" s="1"/>
       <c r="W80" s="1"/>
+      <c r="X80" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactoring: SHKXMLResponseParser now creates proper NSDictionary with nested objects. Preserves original xml structure. Before it flattened the structure to contain all (even nested) elements in the root
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="59">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -309,6 +309,18 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>Delicious</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>shared</t>
   </si>
 </sst>
 </file>
@@ -404,8 +416,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -483,7 +497,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -505,6 +519,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -526,6 +541,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -857,10 +873,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4160" topLeftCell="A26"/>
-      <selection activeCell="E7" sqref="E7"/>
-      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="3560" topLeftCell="A37" activePane="bottomLeft"/>
+      <selection sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="Q64" sqref="Q64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1014,6 +1030,9 @@
       <c r="P14" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="Q14" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:25" s="9" customFormat="1">
       <c r="A15" s="6" t="s">
@@ -1092,7 +1111,9 @@
         <v>5</v>
       </c>
       <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
+      <c r="Q16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -1213,7 +1234,9 @@
         <v>5</v>
       </c>
       <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
+      <c r="Q19" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
@@ -1258,7 +1281,9 @@
         <v>5</v>
       </c>
       <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="Q20" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -1297,7 +1322,9 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
+      <c r="Q21" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -1397,7 +1424,9 @@
         <v>48</v>
       </c>
       <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
+      <c r="Q24" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -1492,7 +1521,9 @@
       <c r="P27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q27" s="8"/>
+      <c r="Q27" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
@@ -1919,7 +1950,9 @@
       <c r="P39" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q39" s="8"/>
+      <c r="Q39" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
       <c r="T39" s="8"/>
@@ -2334,7 +2367,9 @@
         <v>27</v>
       </c>
       <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
+      <c r="Q51" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="R51" s="8"/>
       <c r="S51" s="8"/>
       <c r="T51" s="8"/>
@@ -2746,12 +2781,14 @@
         <v>27</v>
       </c>
       <c r="O63" s="8" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="P63" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q63" s="8"/>
+      <c r="Q63" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="R63" s="8"/>
       <c r="S63" s="8"/>
       <c r="T63" s="8"/>

</xml_diff>

<commit_message>
NEW FEATURE: SHKFlickr can share file - thus preserves exif info. Got rid of ObjectiveFlickr dependency.
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="440" windowWidth="25600" windowHeight="20040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="65">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -321,6 +321,24 @@
   </si>
   <si>
     <t>shared</t>
+  </si>
+  <si>
+    <t>Flickr</t>
+  </si>
+  <si>
+    <t>is_public</t>
+  </si>
+  <si>
+    <t>is_friend</t>
+  </si>
+  <si>
+    <t>is_family</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
 </sst>
 </file>
@@ -416,8 +434,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -497,7 +519,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -520,6 +542,8 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -542,6 +566,8 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -871,12 +897,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y80"/>
+  <dimension ref="A1:Y82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="3560" topLeftCell="A37" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="3140" ySplit="1760" topLeftCell="C30" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="Q64" sqref="Q64"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63:XFD63"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomRight" activeCell="R66" sqref="R66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1033,6 +1061,9 @@
       <c r="Q14" s="5" t="s">
         <v>55</v>
       </c>
+      <c r="R14" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="15" spans="1:25" s="9" customFormat="1">
       <c r="A15" s="6" t="s">
@@ -1058,7 +1089,9 @@
         <v>27</v>
       </c>
       <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
+      <c r="R15" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
@@ -1524,7 +1557,9 @@
       <c r="Q27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="R27" s="8"/>
+      <c r="R27" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
       <c r="U27" s="8"/>
@@ -2067,7 +2102,9 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
+      <c r="R42" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
@@ -2113,7 +2150,9 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
+      <c r="R43" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
@@ -2143,7 +2182,9 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
+      <c r="R44" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
@@ -2181,7 +2222,9 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
+      <c r="R45" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
@@ -2268,7 +2311,9 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
+      <c r="R48" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
@@ -2297,7 +2342,9 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
+      <c r="R49" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
@@ -2322,7 +2369,9 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
+      <c r="R50" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
@@ -2330,104 +2379,103 @@
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
     </row>
-    <row r="51" spans="1:24" s="9" customFormat="1">
-      <c r="A51" s="6" t="s">
+    <row r="51" spans="1:24">
+      <c r="B51" s="3"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+    </row>
+    <row r="52" spans="1:24" s="9" customFormat="1">
+      <c r="A52" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="8" t="s">
+      <c r="B52" s="7"/>
+      <c r="C52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="G52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="H52" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I51" s="8" t="s">
+      <c r="I52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="8" t="s">
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O51" s="8" t="s">
+      <c r="O52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P51" s="8"/>
-      <c r="Q51" s="8" t="s">
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="R51" s="8"/>
-      <c r="S51" s="8"/>
-      <c r="T51" s="8"/>
-      <c r="U51" s="8"/>
-      <c r="V51" s="8"/>
-      <c r="W51" s="8"/>
-      <c r="X51" s="8"/>
-    </row>
-    <row r="52" spans="1:24">
-      <c r="A52" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
-      <c r="S52" s="1"/>
-      <c r="T52" s="1"/>
-      <c r="U52" s="1"/>
-      <c r="V52" s="1"/>
-      <c r="W52" s="1"/>
-      <c r="X52" s="1"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
     </row>
     <row r="53" spans="1:24">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
+      <c r="E53" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="G53" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
+      <c r="M53" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
@@ -2442,7 +2490,7 @@
     </row>
     <row r="54" spans="1:24">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="1"/>
@@ -2455,9 +2503,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
-      <c r="M54" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
@@ -2472,39 +2518,29 @@
     </row>
     <row r="55" spans="1:24">
       <c r="A55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B55" s="3"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
-      <c r="J55" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1" t="s">
         <v>5</v>
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
-      <c r="P55" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
+      <c r="R55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
@@ -2514,21 +2550,27 @@
     </row>
     <row r="56" spans="1:24">
       <c r="A56" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
+      <c r="G56" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="L56" s="1"/>
       <c r="M56" s="1" t="s">
@@ -2537,10 +2579,12 @@
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
+      <c r="R56" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
@@ -2550,33 +2594,35 @@
     </row>
     <row r="57" spans="1:24">
       <c r="A57" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B57" s="3"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
+      <c r="J57" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
+      <c r="M57" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
+      <c r="R57" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
@@ -2586,41 +2632,35 @@
     </row>
     <row r="58" spans="1:24">
       <c r="A58" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
-      <c r="J58" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
       <c r="P58" s="1" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
+      <c r="R58" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
@@ -2629,23 +2669,44 @@
       <c r="X58" s="1"/>
     </row>
     <row r="59" spans="1:24">
-      <c r="B59" s="3"/>
+      <c r="A59" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
+      <c r="E59" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
+      <c r="G59" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
+      <c r="J59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
+      <c r="P59" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
+      <c r="R59" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
@@ -2654,12 +2715,7 @@
       <c r="X59" s="1"/>
     </row>
     <row r="60" spans="1:24">
-      <c r="A60" t="s">
-        <v>20</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="B60" s="3"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -2673,9 +2729,7 @@
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
-      <c r="P60" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
@@ -2686,8 +2740,11 @@
       <c r="X60" s="1"/>
     </row>
     <row r="61" spans="1:24">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
       <c r="B61" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2702,9 +2759,13 @@
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
+      <c r="P61" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
+      <c r="R61" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
@@ -2713,7 +2774,9 @@
       <c r="X61" s="1"/>
     </row>
     <row r="62" spans="1:24">
-      <c r="B62" s="3"/>
+      <c r="B62" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2729,7 +2792,9 @@
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
+      <c r="R62" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
@@ -2737,65 +2802,32 @@
       <c r="W62" s="1"/>
       <c r="X62" s="1"/>
     </row>
-    <row r="63" spans="1:24" s="9" customFormat="1">
-      <c r="A63" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F63" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G63" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H63" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I63" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J63" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K63" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L63" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O63" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="P63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R63" s="8"/>
-      <c r="S63" s="8"/>
-      <c r="T63" s="8"/>
-      <c r="U63" s="8"/>
-      <c r="V63" s="8"/>
-      <c r="W63" s="8"/>
-      <c r="X63" s="8"/>
+    <row r="63" spans="1:24">
+      <c r="B63" s="3"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
     </row>
     <row r="64" spans="1:24">
       <c r="B64" s="3"/>
@@ -2814,7 +2846,9 @@
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
+      <c r="R64" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
@@ -2822,32 +2856,69 @@
       <c r="W64" s="1"/>
       <c r="X64" s="1"/>
     </row>
-    <row r="65" spans="2:24">
-      <c r="B65" s="3"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
-      <c r="S65" s="1"/>
-      <c r="T65" s="1"/>
-      <c r="U65" s="1"/>
-      <c r="V65" s="1"/>
-      <c r="W65" s="1"/>
-      <c r="X65" s="1"/>
-    </row>
-    <row r="66" spans="2:24">
+    <row r="65" spans="1:24" s="9" customFormat="1">
+      <c r="A65" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J65" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K65" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L65" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M65" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N65" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O65" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P65" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q65" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R65" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S65" s="8"/>
+      <c r="T65" s="8"/>
+      <c r="U65" s="8"/>
+      <c r="V65" s="8"/>
+      <c r="W65" s="8"/>
+      <c r="X65" s="8"/>
+    </row>
+    <row r="66" spans="1:24">
       <c r="B66" s="3"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2872,7 +2943,7 @@
       <c r="W66" s="1"/>
       <c r="X66" s="1"/>
     </row>
-    <row r="67" spans="2:24">
+    <row r="67" spans="1:24">
       <c r="B67" s="3"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2897,7 +2968,7 @@
       <c r="W67" s="1"/>
       <c r="X67" s="1"/>
     </row>
-    <row r="68" spans="2:24">
+    <row r="68" spans="1:24">
       <c r="B68" s="3"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2922,7 +2993,7 @@
       <c r="W68" s="1"/>
       <c r="X68" s="1"/>
     </row>
-    <row r="69" spans="2:24">
+    <row r="69" spans="1:24">
       <c r="B69" s="3"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2947,7 +3018,7 @@
       <c r="W69" s="1"/>
       <c r="X69" s="1"/>
     </row>
-    <row r="70" spans="2:24">
+    <row r="70" spans="1:24">
       <c r="B70" s="3"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2972,7 +3043,7 @@
       <c r="W70" s="1"/>
       <c r="X70" s="1"/>
     </row>
-    <row r="71" spans="2:24">
+    <row r="71" spans="1:24">
       <c r="B71" s="3"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -2997,7 +3068,7 @@
       <c r="W71" s="1"/>
       <c r="X71" s="1"/>
     </row>
-    <row r="72" spans="2:24">
+    <row r="72" spans="1:24">
       <c r="B72" s="3"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -3022,7 +3093,7 @@
       <c r="W72" s="1"/>
       <c r="X72" s="1"/>
     </row>
-    <row r="73" spans="2:24">
+    <row r="73" spans="1:24">
       <c r="B73" s="3"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -3047,7 +3118,7 @@
       <c r="W73" s="1"/>
       <c r="X73" s="1"/>
     </row>
-    <row r="74" spans="2:24">
+    <row r="74" spans="1:24">
       <c r="B74" s="3"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -3072,7 +3143,7 @@
       <c r="W74" s="1"/>
       <c r="X74" s="1"/>
     </row>
-    <row r="75" spans="2:24">
+    <row r="75" spans="1:24">
       <c r="B75" s="3"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -3097,7 +3168,7 @@
       <c r="W75" s="1"/>
       <c r="X75" s="1"/>
     </row>
-    <row r="76" spans="2:24">
+    <row r="76" spans="1:24">
       <c r="B76" s="3"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -3122,7 +3193,7 @@
       <c r="W76" s="1"/>
       <c r="X76" s="1"/>
     </row>
-    <row r="77" spans="2:24">
+    <row r="77" spans="1:24">
       <c r="B77" s="3"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -3147,7 +3218,7 @@
       <c r="W77" s="1"/>
       <c r="X77" s="1"/>
     </row>
-    <row r="78" spans="2:24">
+    <row r="78" spans="1:24">
       <c r="B78" s="3"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -3172,7 +3243,7 @@
       <c r="W78" s="1"/>
       <c r="X78" s="1"/>
     </row>
-    <row r="79" spans="2:24">
+    <row r="79" spans="1:24">
       <c r="B79" s="3"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3197,7 +3268,7 @@
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
     </row>
-    <row r="80" spans="2:24">
+    <row r="80" spans="1:24">
       <c r="B80" s="3"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -3222,6 +3293,56 @@
       <c r="W80" s="1"/>
       <c r="X80" s="1"/>
     </row>
+    <row r="81" spans="2:24">
+      <c r="B81" s="3"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="1"/>
+      <c r="U81" s="1"/>
+      <c r="V81" s="1"/>
+      <c r="W81" s="1"/>
+      <c r="X81" s="1"/>
+    </row>
+    <row r="82" spans="2:24">
+      <c r="B82" s="3"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="1"/>
+      <c r="U82" s="1"/>
+      <c r="V82" s="1"/>
+      <c r="W82" s="1"/>
+      <c r="X82" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
NEW FEATURE: Flickr supports video
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="64">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -336,9 +336,6 @@
   </si>
   <si>
     <t>groups</t>
-  </si>
-  <si>
-    <t>image</t>
   </si>
 </sst>
 </file>
@@ -900,11 +897,11 @@
   <dimension ref="A1:Y82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="3140" ySplit="1760" topLeftCell="C30" activePane="bottomRight"/>
+      <pane xSplit="3140" ySplit="1760" topLeftCell="E43" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
+      <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="A63" sqref="A63:XFD63"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomRight" activeCell="R66" sqref="R66"/>
+      <selection pane="bottomRight" activeCell="R60" sqref="R60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2705,7 +2702,7 @@
       </c>
       <c r="Q59" s="1"/>
       <c r="R59" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>

</xml_diff>

<commit_message>
BUGFIX: iOS sharer native iOS UI can not fetch user info - now the sharer does not try to use SLComposeViewController for this. BUGFIX: demo app accounts view now shows only sharers who can share, and require authorisation DOCUMENTATION: updated sharer matrix
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -24,7 +24,7 @@
     <author>Vilém Kurz</author>
   </authors>
   <commentList>
-    <comment ref="N19" authorId="0">
+    <comment ref="N21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0">
+    <comment ref="B22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N20" authorId="0">
+    <comment ref="N22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="66">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>groups</t>
+  </si>
+  <si>
+    <t>item.URLPictureURI</t>
+  </si>
+  <si>
+    <t>item.URLDescription</t>
   </si>
 </sst>
 </file>
@@ -894,14 +900,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y82"/>
+  <dimension ref="A1:Y84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="3140" ySplit="1760" topLeftCell="E43" activePane="bottomRight"/>
+      <pane xSplit="3140" ySplit="1760" topLeftCell="A8" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63:XFD63"/>
-      <selection pane="bottomRight" activeCell="R60" sqref="R60"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1184,34 +1190,30 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" ht="18" customHeight="1">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="L18" s="1"/>
-      <c r="M18" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="O18" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -1223,50 +1225,32 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" ht="18" customHeight="1">
       <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
       <c r="O19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="P19" s="1"/>
-      <c r="Q19" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
@@ -1278,42 +1262,34 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -1325,13 +1301,15 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1345,15 +1323,25 @@
       <c r="I21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="M21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -1366,30 +1354,42 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+      <c r="N22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
+      <c r="Q22" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
@@ -1400,14 +1400,27 @@
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="1:25">
-      <c r="B23" s="3"/>
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1415,7 +1428,9 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="Q23" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
@@ -1427,36 +1442,30 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B24" s="3"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="M24" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N24" s="1"/>
-      <c r="O24" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -1467,24 +1476,16 @@
       <c r="Y24" s="1"/>
     </row>
     <row r="25" spans="1:25">
-      <c r="B25" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="B25" s="3"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1501,9 +1502,16 @@
       <c r="Y25" s="1"/>
     </row>
     <row r="26" spans="1:25">
-      <c r="B26" s="3"/>
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1514,9 +1522,13 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
+      <c r="O26" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
+      <c r="Q26" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
@@ -1526,74 +1538,49 @@
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
     </row>
-    <row r="27" spans="1:25" s="9" customFormat="1">
-      <c r="A27" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q27" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R27" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="8"/>
-      <c r="W27" s="8"/>
-      <c r="X27" s="8"/>
+    <row r="27" spans="1:25">
+      <c r="B27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
     </row>
     <row r="28" spans="1:25">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
       <c r="B28" s="3"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1605,38 +1592,49 @@
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
-    </row>
-    <row r="29" spans="1:25">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
+      <c r="Y28" s="1"/>
+    </row>
+    <row r="29" spans="1:25" s="9" customFormat="1">
+      <c r="A29" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
     </row>
     <row r="30" spans="1:25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="1"/>
@@ -1654,8 +1652,12 @@
       <c r="I30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
+      <c r="J30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1" t="s">
         <v>5</v>
@@ -1674,11 +1676,9 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B31" s="3"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1686,16 +1686,10 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1710,15 +1704,11 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B32" s="3"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1728,28 +1718,18 @@
       <c r="G32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -1762,30 +1742,28 @@
     </row>
     <row r="33" spans="1:24">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="M33" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -1800,28 +1778,46 @@
     </row>
     <row r="34" spans="1:24">
       <c r="A34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
+      <c r="N34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
@@ -1833,14 +1829,27 @@
       <c r="X34" s="1"/>
     </row>
     <row r="35" spans="1:24">
-      <c r="B35" s="3"/>
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1859,32 +1868,28 @@
     </row>
     <row r="36" spans="1:24">
       <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="G36" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
+      <c r="M36" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N36" s="1"/>
-      <c r="O36" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
@@ -1896,24 +1901,16 @@
       <c r="X36" s="1"/>
     </row>
     <row r="37" spans="1:24">
-      <c r="B37" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="B37" s="3"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K37" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -1929,20 +1926,33 @@
       <c r="X37" s="1"/>
     </row>
     <row r="38" spans="1:24">
-      <c r="B38" s="3"/>
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
+      <c r="J38" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
+      <c r="O38" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
@@ -1953,72 +1963,52 @@
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
     </row>
-    <row r="39" spans="1:24" s="9" customFormat="1">
-      <c r="A39" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O39" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P39" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q39" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
+    <row r="39" spans="1:24">
+      <c r="B39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
     </row>
     <row r="40" spans="1:24">
-      <c r="A40" t="s">
-        <v>7</v>
-      </c>
       <c r="B40" s="3"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J40" s="10"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -2031,45 +2021,53 @@
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
     </row>
-    <row r="41" spans="1:24">
-      <c r="A41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
-      <c r="W41" s="1"/>
-      <c r="X41" s="1"/>
+    <row r="41" spans="1:24" s="9" customFormat="1">
+      <c r="A41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
     </row>
     <row r="42" spans="1:24">
       <c r="A42" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B42" s="3"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
         <v>5</v>
       </c>
@@ -2083,15 +2081,9 @@
       <c r="I42" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J42" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="J42" s="10"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
       <c r="M42" s="1" t="s">
         <v>5</v>
       </c>
@@ -2099,9 +2091,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
-      <c r="R42" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
@@ -2111,45 +2101,25 @@
     </row>
     <row r="43" spans="1:24">
       <c r="A43" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B43" s="3"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J43" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
-      <c r="R43" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
@@ -2159,19 +2129,37 @@
     </row>
     <row r="44" spans="1:24">
       <c r="A44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
+      <c r="I44" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M44" s="1" t="s">
         <v>5</v>
       </c>
@@ -2180,7 +2168,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
@@ -2191,30 +2179,38 @@
     </row>
     <row r="45" spans="1:24">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G45" s="1" t="s">
+      <c r="F45" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
+      <c r="I45" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
+      <c r="M45" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
@@ -2231,7 +2227,7 @@
     </row>
     <row r="46" spans="1:24">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="1"/>
@@ -2251,7 +2247,9 @@
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
+      <c r="R46" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
@@ -2260,14 +2258,27 @@
       <c r="X46" s="1"/>
     </row>
     <row r="47" spans="1:24">
-      <c r="B47" s="3"/>
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
+      <c r="I47" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -2276,7 +2287,9 @@
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
+      <c r="R47" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
@@ -2286,15 +2299,11 @@
     </row>
     <row r="48" spans="1:24">
       <c r="A48" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B48" s="3"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -2303,14 +2312,14 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
+      <c r="M48" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
-      <c r="R48" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="R48" s="1"/>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
@@ -2319,13 +2328,9 @@
       <c r="X48" s="1"/>
     </row>
     <row r="49" spans="1:24">
-      <c r="B49" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="B49" s="3"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2339,9 +2344,7 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
-      <c r="R49" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="R49" s="1"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
@@ -2350,9 +2353,16 @@
       <c r="X49" s="1"/>
     </row>
     <row r="50" spans="1:24">
-      <c r="B50" s="3"/>
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -2367,7 +2377,7 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
@@ -2377,9 +2387,13 @@
       <c r="X50" s="1"/>
     </row>
     <row r="51" spans="1:24">
-      <c r="B51" s="3"/>
+      <c r="B51" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -2394,7 +2408,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
@@ -2403,81 +2417,53 @@
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
     </row>
-    <row r="52" spans="1:24" s="9" customFormat="1">
-      <c r="A52" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="8"/>
-      <c r="N52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P52" s="8"/>
-      <c r="Q52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R52" s="8"/>
-      <c r="S52" s="8"/>
-      <c r="T52" s="8"/>
-      <c r="U52" s="8"/>
-      <c r="V52" s="8"/>
-      <c r="W52" s="8"/>
-      <c r="X52" s="8"/>
+    <row r="52" spans="1:24">
+      <c r="B52" s="3"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
     </row>
     <row r="53" spans="1:24">
-      <c r="A53" t="s">
-        <v>7</v>
-      </c>
       <c r="B53" s="3"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
-      <c r="M53" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
+      <c r="R53" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
@@ -2485,44 +2471,68 @@
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
     </row>
-    <row r="54" spans="1:24">
-      <c r="A54" t="s">
-        <v>8</v>
-      </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
-      <c r="S54" s="1"/>
-      <c r="T54" s="1"/>
-      <c r="U54" s="1"/>
-      <c r="V54" s="1"/>
-      <c r="W54" s="1"/>
-      <c r="X54" s="1"/>
+    <row r="54" spans="1:24" s="9" customFormat="1">
+      <c r="A54" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="7"/>
+      <c r="C54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R54" s="8"/>
+      <c r="S54" s="8"/>
+      <c r="T54" s="8"/>
+      <c r="U54" s="8"/>
+      <c r="V54" s="8"/>
+      <c r="W54" s="8"/>
+      <c r="X54" s="8"/>
     </row>
     <row r="55" spans="1:24">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+      <c r="G55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
@@ -2535,9 +2545,7 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
-      <c r="R55" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="R55" s="1"/>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
@@ -2547,41 +2555,25 @@
     </row>
     <row r="56" spans="1:24">
       <c r="A56" t="s">
-        <v>9</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B56" s="3"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
-      <c r="J56" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
       <c r="L56" s="1"/>
-      <c r="M56" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
-      <c r="P56" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
-      <c r="R56" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="R56" s="1"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
@@ -2591,7 +2583,7 @@
     </row>
     <row r="57" spans="1:24">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="1"/>
@@ -2601,24 +2593,18 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
-      <c r="J57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
-      <c r="P57" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="1" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
@@ -2629,7 +2615,7 @@
     </row>
     <row r="58" spans="1:24">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>5</v>
@@ -2645,10 +2631,16 @@
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
+      <c r="J58" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
+      <c r="M58" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
       <c r="P58" s="1" t="s">
@@ -2667,42 +2659,34 @@
     </row>
     <row r="59" spans="1:24">
       <c r="A59" t="s">
-        <v>39</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B59" s="3"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-      <c r="G59" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="L59" s="1"/>
       <c r="M59" s="1" t="s">
         <v>5</v>
       </c>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Q59" s="1"/>
       <c r="R59" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
@@ -2712,12 +2696,21 @@
       <c r="X59" s="1"/>
     </row>
     <row r="60" spans="1:24">
-      <c r="B60" s="3"/>
+      <c r="A60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
+      <c r="E60" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
+      <c r="G60" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
@@ -2726,9 +2719,13 @@
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
+      <c r="P60" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
+      <c r="R60" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
@@ -2738,30 +2735,42 @@
     </row>
     <row r="61" spans="1:24">
       <c r="A61" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
+      <c r="E61" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
+      <c r="G61" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
+      <c r="J61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
       <c r="P61" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="Q61" s="1"/>
       <c r="R61" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
@@ -2771,9 +2780,7 @@
       <c r="X61" s="1"/>
     </row>
     <row r="62" spans="1:24">
-      <c r="B62" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="B62" s="3"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2789,9 +2796,7 @@
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
-      <c r="R62" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="R62" s="1"/>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
@@ -2800,7 +2805,12 @@
       <c r="X62" s="1"/>
     </row>
     <row r="63" spans="1:24">
-      <c r="B63" s="3"/>
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -2814,10 +2824,12 @@
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
+      <c r="P63" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="Q63" s="1"/>
       <c r="R63" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
@@ -2827,7 +2839,9 @@
       <c r="X63" s="1"/>
     </row>
     <row r="64" spans="1:24">
-      <c r="B64" s="3"/>
+      <c r="B64" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -2844,7 +2858,7 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
@@ -2853,67 +2867,32 @@
       <c r="W64" s="1"/>
       <c r="X64" s="1"/>
     </row>
-    <row r="65" spans="1:24" s="9" customFormat="1">
-      <c r="A65" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F65" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G65" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H65" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I65" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J65" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K65" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L65" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M65" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N65" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O65" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="P65" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q65" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R65" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="S65" s="8"/>
-      <c r="T65" s="8"/>
-      <c r="U65" s="8"/>
-      <c r="V65" s="8"/>
-      <c r="W65" s="8"/>
-      <c r="X65" s="8"/>
+    <row r="65" spans="1:24">
+      <c r="B65" s="3"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
     </row>
     <row r="66" spans="1:24">
       <c r="B66" s="3"/>
@@ -2932,7 +2911,9 @@
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
+      <c r="R66" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
@@ -2940,30 +2921,67 @@
       <c r="W66" s="1"/>
       <c r="X66" s="1"/>
     </row>
-    <row r="67" spans="1:24">
-      <c r="B67" s="3"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
+    <row r="67" spans="1:24" s="9" customFormat="1">
+      <c r="A67" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J67" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K67" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L67" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O67" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R67" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S67" s="8"/>
+      <c r="T67" s="8"/>
+      <c r="U67" s="8"/>
+      <c r="V67" s="8"/>
+      <c r="W67" s="8"/>
+      <c r="X67" s="8"/>
     </row>
     <row r="68" spans="1:24">
       <c r="B68" s="3"/>
@@ -3340,6 +3358,56 @@
       <c r="W82" s="1"/>
       <c r="X82" s="1"/>
     </row>
+    <row r="83" spans="2:24">
+      <c r="B83" s="3"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="1"/>
+      <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+      <c r="W83" s="1"/>
+      <c r="X83" s="1"/>
+    </row>
+    <row r="84" spans="2:24">
+      <c r="B84" s="3"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+      <c r="S84" s="1"/>
+      <c r="T84" s="1"/>
+      <c r="U84" s="1"/>
+      <c r="V84" s="1"/>
+      <c r="W84" s="1"/>
+      <c r="X84" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
NEW FEATURE: google+ image and video share
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Vilém Kurz</author>
+    <author>Vilem Kurz</author>
   </authors>
   <commentList>
     <comment ref="N21" authorId="0">
@@ -96,12 +97,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="H67" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Vilem Kurz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+You can get user info via[ [GPPSignIn sharedInstance] googlePlusUser]</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="66">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -903,11 +928,11 @@
   <dimension ref="A1:Y84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="3140" ySplit="1760" topLeftCell="A8" activePane="bottomRight"/>
+      <pane xSplit="3140" ySplit="1760" topLeftCell="A33" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="O27" sqref="O27"/>
+      <selection pane="bottomRight" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2033,9 +2058,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="11" t="s">
-        <v>27</v>
-      </c>
+      <c r="H41" s="11"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
@@ -2147,7 +2170,9 @@
       <c r="G44" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="I44" s="10" t="s">
         <v>5</v>
       </c>
@@ -2235,7 +2260,9 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
+      <c r="H46" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
@@ -2667,7 +2694,9 @@
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
+      <c r="H59" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1" t="s">
         <v>37</v>
@@ -2749,7 +2778,9 @@
       <c r="G61" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H61" s="1"/>
+      <c r="H61" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1" t="s">
         <v>40</v>
@@ -2944,7 +2975,7 @@
         <v>5</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="I67" s="11" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
NEW FEATURE: SHKDropbox can get user info
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19440" tabRatio="500"/>
@@ -932,7 +932,7 @@
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="H71" sqref="H71"/>
+      <selection pane="bottomRight" activeCell="L68" sqref="L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2987,7 +2987,7 @@
         <v>5</v>
       </c>
       <c r="L67" s="11" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="M67" s="8" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
BUGFIX: TextMessage sharer accepts also title. Updated documentation.
</commit_message>
<xml_diff>
--- a/Documentation/sharer_itemProperty_support_matrix.xlsx
+++ b/Documentation/sharer_itemProperty_support_matrix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19440" tabRatio="500"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="67">
   <si>
     <t>SHKShareTypeURL</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>item.URLDescription</t>
+  </si>
+  <si>
+    <t>Text Message</t>
   </si>
 </sst>
 </file>
@@ -462,8 +465,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -547,7 +562,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -572,6 +587,12 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -596,6 +617,12 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -928,11 +955,11 @@
   <dimension ref="A1:Y84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="3140" ySplit="1760" topLeftCell="A33" activePane="bottomRight"/>
+      <pane xSplit="3140" ySplit="1760" topLeftCell="D32" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="L68" sqref="L68"/>
+      <selection pane="bottomRight" activeCell="S57" sqref="S57:S61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1092,6 +1119,9 @@
       <c r="R14" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="S14" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="15" spans="1:25" s="9" customFormat="1">
       <c r="A15" s="6" t="s">
@@ -1176,7 +1206,9 @@
         <v>5</v>
       </c>
       <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
+      <c r="S16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
@@ -1316,7 +1348,9 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
+      <c r="S20" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
@@ -1369,7 +1403,9 @@
         <v>56</v>
       </c>
       <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
+      <c r="S21" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
@@ -1416,7 +1452,9 @@
         <v>57</v>
       </c>
       <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
+      <c r="S22" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
@@ -1492,7 +1530,9 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
+      <c r="S24" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
@@ -1692,7 +1732,9 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
+      <c r="S30" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
@@ -1758,7 +1800,9 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
+      <c r="S32" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
@@ -1794,7 +1838,9 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
+      <c r="S33" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
@@ -1846,7 +1892,9 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
+      <c r="S34" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
@@ -1918,7 +1966,9 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
+      <c r="S36" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
@@ -1943,7 +1993,6 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -1981,7 +2030,6 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
@@ -2115,7 +2163,9 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
+      <c r="S42" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
@@ -2195,7 +2245,9 @@
       <c r="R44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S44" s="1"/>
+      <c r="S44" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
@@ -2243,7 +2295,9 @@
       <c r="R45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S45" s="1"/>
+      <c r="S45" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
       <c r="V45" s="1"/>
@@ -2277,7 +2331,9 @@
       <c r="R46" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="S46" s="1"/>
+      <c r="S46" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
@@ -2347,7 +2403,9 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
+      <c r="S48" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
       <c r="V48" s="1"/>
@@ -2372,7 +2430,6 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
       <c r="V49" s="1"/>
@@ -2406,7 +2463,6 @@
       <c r="R50" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="S50" s="1"/>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
       <c r="V50" s="1"/>
@@ -2573,7 +2629,9 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
-      <c r="S55" s="1"/>
+      <c r="S55" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
       <c r="V55" s="1"/>
@@ -2633,7 +2691,9 @@
       <c r="R57" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S57" s="1"/>
+      <c r="S57" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
       <c r="V57" s="1"/>
@@ -2677,7 +2737,9 @@
       <c r="R58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S58" s="1"/>
+      <c r="S58" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
       <c r="V58" s="1"/>
@@ -2717,7 +2779,9 @@
       <c r="R59" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="S59" s="1"/>
+      <c r="S59" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
       <c r="V59" s="1"/>
@@ -2803,7 +2867,9 @@
       <c r="R61" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S61" s="1"/>
+      <c r="S61" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
       <c r="V61" s="1"/>
@@ -2828,7 +2894,6 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
-      <c r="S62" s="1"/>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
       <c r="V62" s="1"/>
@@ -2862,7 +2927,6 @@
       <c r="R63" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="S63" s="1"/>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
       <c r="V63" s="1"/>
@@ -3007,7 +3071,9 @@
       <c r="R67" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="S67" s="8"/>
+      <c r="S67" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="T67" s="8"/>
       <c r="U67" s="8"/>
       <c r="V67" s="8"/>

</xml_diff>